<commit_message>
Add some visualization. Fix bugs. Fix logs
</commit_message>
<xml_diff>
--- a/server/res/blockInfo.xlsx
+++ b/server/res/blockInfo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>textureOffsety</t>
+  </si>
+  <si>
+    <t>multiTexture</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>spike</t>
   </si>
 </sst>
 </file>
@@ -425,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,7 +445,7 @@
     <col min="1" max="11" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +476,14 @@
       <c r="J1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -499,8 +514,14 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -531,8 +552,14 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -563,8 +590,14 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -595,8 +628,14 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -627,8 +666,14 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -659,8 +704,14 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -691,8 +742,14 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -723,8 +780,14 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -755,8 +818,14 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -787,8 +856,14 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -818,6 +893,50 @@
       </c>
       <c r="J12" s="1">
         <v>-195</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>